<commit_message>
update test sheet to 1 file only, add TS delete customer and add script good method for filtering and verify delete
</commit_message>
<xml_diff>
--- a/Data Files/Test Data/List Customer Name.xlsx
+++ b/Data Files/Test Data/List Customer Name.xlsx
@@ -3,7 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId5"/>
+    <sheet state="visible" name="List Name" sheetId="1" r:id="rId5"/>
+    <sheet state="visible" name="New Customer" sheetId="2" r:id="rId6"/>
+    <sheet state="visible" name="Delete Customer" sheetId="3" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>CustomerName</t>
   </si>
@@ -29,13 +31,49 @@
   </si>
   <si>
     <t>Neville Longbottom</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Postode</t>
+  </si>
+  <si>
+    <t>Putra</t>
+  </si>
+  <si>
+    <t>Alrasy</t>
+  </si>
+  <si>
+    <t>Lee</t>
+  </si>
+  <si>
+    <t>Chong</t>
+  </si>
+  <si>
+    <t>Ali</t>
+  </si>
+  <si>
+    <t>Muthu</t>
+  </si>
+  <si>
+    <t>customerName</t>
+  </si>
+  <si>
+    <t>Harry</t>
+  </si>
+  <si>
+    <t>Ron</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -46,6 +84,10 @@
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -62,12 +104,18 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -78,6 +126,14 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -322,4 +378,93 @@
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="3">
+        <v>81200.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="3">
+        <v>50000.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="3">
+        <v>64570.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>